<commit_message>
add function main() to make code reusable
</commit_message>
<xml_diff>
--- a/New_ID.xlsx
+++ b/New_ID.xlsx
@@ -14,21 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Новий ID:</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>4</t>
+    <t>7VlJ2</t>
+  </si>
+  <si>
+    <t>2DtB3</t>
+  </si>
+  <si>
+    <t>3EtC2</t>
+  </si>
+  <si>
+    <t>5SbY2</t>
+  </si>
+  <si>
+    <t>9YmO4</t>
   </si>
 </sst>
 </file>
@@ -369,7 +372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -400,6 +403,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding enumerate() and generate_id()
</commit_message>
<xml_diff>
--- a/New_ID.xlsx
+++ b/New_ID.xlsx
@@ -14,24 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Новий ID:</t>
   </si>
   <si>
-    <t>7VlJ2</t>
+    <t>1YwE0</t>
   </si>
   <si>
-    <t>2DtB3</t>
-  </si>
-  <si>
-    <t>3EtC2</t>
-  </si>
-  <si>
-    <t>5SbY2</t>
-  </si>
-  <si>
-    <t>9YmO4</t>
+    <t>9LcF2</t>
   </si>
 </sst>
 </file>
@@ -372,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -393,21 +384,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added changes according to test3
</commit_message>
<xml_diff>
--- a/New_ID.xlsx
+++ b/New_ID.xlsx
@@ -19,10 +19,10 @@
     <t>Новий ID:</t>
   </si>
   <si>
-    <t>1YwE0</t>
+    <t>3RdW7</t>
   </si>
   <si>
-    <t>9LcF2</t>
+    <t>6LyT6</t>
   </si>
 </sst>
 </file>

</xml_diff>